<commit_message>
update excel read and write to use versions
</commit_message>
<xml_diff>
--- a/excel_sheets/Indicator_metadata.xlsx
+++ b/excel_sheets/Indicator_metadata.xlsx
@@ -507,7 +507,7 @@
       <c r="B1" s="2" t="n"/>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>indicator type metadata version 0.1.0</t>
+          <t>metadata_type: indicator, metadata_type_version: 0.1.0</t>
         </is>
       </c>
       <c r="D1" s="2" t="n"/>
@@ -4148,9 +4148,7 @@
           <t>adjustments</t>
         </is>
       </c>
-      <c r="C24" s="6" t="n">
-        <v/>
-      </c>
+      <c r="C24" s="6" t="n"/>
       <c r="D24" s="6" t="n"/>
       <c r="E24" s="6" t="n"/>
       <c r="F24" s="6" t="n"/>
@@ -4222,9 +4220,7 @@
           <t>validation_rules</t>
         </is>
       </c>
-      <c r="C26" s="6" t="n">
-        <v/>
-      </c>
+      <c r="C26" s="6" t="n"/>
       <c r="D26" s="6" t="n"/>
       <c r="E26" s="6" t="n"/>
       <c r="F26" s="6" t="n"/>

</xml_diff>